<commit_message>
[feature][FinancialTools][merge] add merge all file and sheets in folder
[what] 合并文件夹下的所有文件的所有工作簿
[why]null
[how]null
</commit_message>
<xml_diff>
--- a/datas/merge/1月.xlsx
+++ b/datas/merge/1月.xlsx
@@ -8,14 +8,15 @@
     <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="55">
   <si>
     <t>科目编号</t>
   </si>
@@ -187,12 +188,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +204,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -224,9 +233,92 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -235,20 +327,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,44 +345,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -312,52 +352,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -368,187 +362,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,26 +571,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,16 +613,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,6 +641,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,147 +668,121 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -803,22 +791,28 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1595,4 +1589,431 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>